<commit_message>
Load data from google sheets
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfnei\Desktop\MUSA-PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B041DC-0726-4AA5-8E14-B4E45FB105A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2627EE-8008-45FA-99C9-A50AAA602F0D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20280" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{9173ABE8-A629-4176-B4CC-FB3DF8ED276C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID-CODE</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>OPERATIONSTEXT-CODE</t>
+  </si>
+  <si>
+    <t>Consulta</t>
+  </si>
+  <si>
+    <t>(fila, columna)</t>
   </si>
 </sst>
 </file>
@@ -166,16 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -186,6 +186,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ADEC022-5F35-43C7-A16A-53868B11173A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,142 +522,151 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="F15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A14:C15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="F2:F12"/>
     <mergeCell ref="G2:G12"/>
     <mergeCell ref="A1:C1"/>
@@ -656,7 +674,6 @@
     <mergeCell ref="A6:C7"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A12:C13"/>
-    <mergeCell ref="A14:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>